<commit_message>
Add "mode" to input Excel setup
</commit_message>
<xml_diff>
--- a/scenario work/add_storage_tech/setup_storage.xlsx
+++ b/scenario work/add_storage_tech/setup_storage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\time_clustering\scenario work\add_storage_tech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A10EDD47-660A-45E2-8B6A-B8304FCA1B0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A733A3-1923-4530-9837-B0AB051ACA3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="19935" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="storage" sheetId="20" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>tc={2A9BC780-3573-49FC-934D-EB88E44ABA62}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{2A9BC780-3573-49FC-934D-EB88E44ABA62}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{2A9BC780-3573-49FC-934D-EB88E44ABA62}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="100">
   <si>
     <t>technology</t>
   </si>
@@ -346,6 +346,12 @@
   </si>
   <si>
     <t>Thermal energy storage in buildings</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>M1</t>
   </si>
 </sst>
 </file>
@@ -624,64 +630,19 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -743,40 +704,40 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -785,6 +746,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1081,7 +1087,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C1" dT="2019-11-26T17:01:21.48" personId="{5B2321EA-5DE5-468C-9F9C-016B7D7F0B1F}" id="{2A9BC780-3573-49FC-934D-EB88E44ABA62}">
+  <threadedComment ref="D1" dT="2019-11-26T17:01:21.48" personId="{5B2321EA-5DE5-468C-9F9C-016B7D7F0B1F}" id="{2A9BC780-3573-49FC-934D-EB88E44ABA62}">
     <text>either 'all' or one string or strings seprated by (/)</text>
   </threadedComment>
 </ThreadedComments>
@@ -1089,35 +1095,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F56DBD-A483-468D-94AB-6D22FF1A0021}">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.85546875" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8" customWidth="1"/>
-    <col min="20" max="20" width="7.42578125" customWidth="1"/>
-    <col min="21" max="21" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
+    <col min="4" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.85546875" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" customWidth="1"/>
+    <col min="22" max="22" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -1125,64 +1132,67 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1190,56 +1200,59 @@
         <v>40</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="5"/>
       <c r="O2" s="5"/>
-      <c r="P2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="86" t="s">
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S2" s="5"/>
       <c r="T2" s="5"/>
-      <c r="U2" s="55" t="s">
+      <c r="U2" s="5"/>
+      <c r="V2" s="157" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1247,58 +1260,61 @@
         <v>37</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="F3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="9"/>
       <c r="O3" s="9"/>
-      <c r="P3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="48" t="s">
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="9">
+      <c r="T3" s="9">
         <v>1</v>
       </c>
-      <c r="T3" s="48">
+      <c r="U3" s="48">
         <v>0.01</v>
       </c>
-      <c r="U3" s="56"/>
+      <c r="V3" s="158"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
@@ -1306,56 +1322,59 @@
         <v>36</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9" t="s">
+      <c r="O4" s="9"/>
+      <c r="P4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" s="48" t="s">
+      <c r="Q4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="S4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="S4" s="9"/>
-      <c r="T4" s="48"/>
-      <c r="U4" s="57"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="159"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
@@ -1363,58 +1382,61 @@
         <v>38</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="I5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>1</v>
+      <c r="L5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="N5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q5" s="49" t="s">
+      <c r="O5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="R5" s="13" t="s">
+      <c r="S5" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="S5" s="13"/>
-      <c r="T5" s="49"/>
-      <c r="U5" s="58" t="s">
+      <c r="T5" s="13"/>
+      <c r="U5" s="49"/>
+      <c r="V5" s="154" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -1422,60 +1444,63 @@
         <v>39</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D6" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="17" t="s">
+      <c r="F6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="17" t="s">
+      <c r="I6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>1</v>
+      <c r="L6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="N6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q6" s="50" t="s">
+      <c r="O6" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="R6" s="17" t="s">
+      <c r="S6" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="S6" s="17">
+      <c r="T6" s="17">
         <v>1</v>
       </c>
-      <c r="T6" s="50">
+      <c r="U6" s="50">
         <v>0.01</v>
       </c>
-      <c r="U6" s="59"/>
+      <c r="V6" s="155"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>8</v>
       </c>
@@ -1483,37 +1508,37 @@
         <v>1</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D7" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="F7" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="21" t="s">
+      <c r="I7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="L7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="M7" s="23" t="s">
         <v>28</v>
-      </c>
-      <c r="M7" s="21" t="s">
-        <v>1</v>
       </c>
       <c r="N7" s="21" t="s">
         <v>1</v>
@@ -1522,19 +1547,22 @@
         <v>1</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="R7" s="21" t="s">
+      <c r="S7" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="S7" s="21"/>
-      <c r="T7" s="51"/>
-      <c r="U7" s="60"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="51"/>
+      <c r="V7" s="156"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>7</v>
       </c>
@@ -1542,58 +1570,61 @@
         <v>41</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D8" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="F8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="I8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="25" t="s">
-        <v>43</v>
+      <c r="L8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="27" t="s">
+        <v>17</v>
       </c>
       <c r="N8" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q8" s="52" t="s">
+      <c r="O8" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="R8" s="25" t="s">
+      <c r="S8" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="S8" s="25"/>
-      <c r="T8" s="52"/>
-      <c r="U8" s="61" t="s">
+      <c r="T8" s="25"/>
+      <c r="U8" s="52"/>
+      <c r="V8" s="151" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>9</v>
       </c>
@@ -1601,60 +1632,63 @@
         <v>42</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D9" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="29" t="s">
+      <c r="F9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="29" t="s">
+      <c r="I9" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="29" t="s">
-        <v>43</v>
+      <c r="L9" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="N9" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q9" s="53" t="s">
+      <c r="O9" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="R9" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="R9" s="29" t="s">
+      <c r="S9" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="S9" s="29">
+      <c r="T9" s="29">
         <v>1</v>
       </c>
-      <c r="T9" s="53">
+      <c r="U9" s="53">
         <v>0.01</v>
       </c>
-      <c r="U9" s="62"/>
+      <c r="V9" s="152"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>8</v>
       </c>
@@ -1662,37 +1696,37 @@
         <v>43</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D10" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="F10" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="33" t="s">
+      <c r="I10" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="33" t="s">
+      <c r="L10" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="M10" s="35" t="s">
         <v>28</v>
-      </c>
-      <c r="M10" s="33" t="s">
-        <v>43</v>
       </c>
       <c r="N10" s="33" t="s">
         <v>43</v>
@@ -1701,19 +1735,22 @@
         <v>43</v>
       </c>
       <c r="P10" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q10" s="87" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q10" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="R10" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="33" t="s">
+      <c r="S10" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="S10" s="33"/>
       <c r="T10" s="33"/>
-      <c r="U10" s="63"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="153"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>7</v>
       </c>
@@ -1721,56 +1758,59 @@
         <v>91</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D11" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="F11" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="F11" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="37" t="s">
+      <c r="I11" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="83" t="s">
+      <c r="J11" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="37" t="s">
+      <c r="K11" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="M11" s="37" t="s">
+      <c r="L11" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="N11" s="37"/>
       <c r="O11" s="37"/>
-      <c r="P11" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q11" s="88" t="s">
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="R11" s="37" t="s">
+      <c r="S11" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="S11" s="37"/>
       <c r="T11" s="37"/>
-      <c r="U11" s="64" t="s">
+      <c r="U11" s="37"/>
+      <c r="V11" s="148" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>9</v>
       </c>
@@ -1778,58 +1818,61 @@
         <v>90</v>
       </c>
       <c r="C12" s="41" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D12" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="41" t="s">
+      <c r="F12" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="41" t="s">
+      <c r="I12" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="K12" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="M12" s="41" t="s">
+      <c r="L12" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="N12" s="41"/>
       <c r="O12" s="41"/>
-      <c r="P12" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q12" s="54" t="s">
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="R12" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="R12" s="41" t="s">
+      <c r="S12" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="S12" s="41">
+      <c r="T12" s="41">
         <v>1</v>
       </c>
-      <c r="T12" s="54">
+      <c r="U12" s="54">
         <v>0.01</v>
       </c>
-      <c r="U12" s="65"/>
+      <c r="V12" s="149"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
         <v>8</v>
       </c>
@@ -1837,925 +1880,973 @@
         <v>92</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="D13" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="F13" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="F13" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="45" t="s">
+      <c r="G13" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="45" t="s">
+      <c r="I13" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="K13" s="45" t="s">
+      <c r="L13" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="L13" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" s="45" t="s">
+      <c r="M13" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="N13" s="45"/>
       <c r="O13" s="45"/>
-      <c r="P13" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q13" s="85" t="s">
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="R13" s="45" t="s">
+      <c r="S13" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="S13" s="45"/>
       <c r="T13" s="45"/>
-      <c r="U13" s="66"/>
+      <c r="U13" s="45"/>
+      <c r="V13" s="150"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="139" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="124" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="140" t="s">
+      <c r="B14" s="125" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="140" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="140" t="s">
+      <c r="C14" s="125" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="125" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="141" t="s">
+      <c r="F14" s="126" t="s">
         <v>94</v>
       </c>
-      <c r="F14" s="142" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="140" t="s">
+      <c r="G14" s="127" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="H14" s="140" t="s">
+      <c r="I14" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="143" t="s">
+      <c r="J14" s="128" t="s">
         <v>46</v>
       </c>
-      <c r="J14" s="140" t="s">
+      <c r="K14" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="K14" s="140" t="s">
-        <v>9</v>
-      </c>
-      <c r="L14" s="143" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14" s="140" t="s">
+      <c r="L14" s="125" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="128" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="N14" s="140"/>
-      <c r="O14" s="140"/>
-      <c r="P14" s="140" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q14" s="140" t="s">
+      <c r="O14" s="125"/>
+      <c r="P14" s="125"/>
+      <c r="Q14" s="125" t="s">
+        <v>29</v>
+      </c>
+      <c r="R14" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="R14" s="140" t="s">
+      <c r="S14" s="125" t="s">
         <v>55</v>
       </c>
-      <c r="S14" s="140"/>
-      <c r="T14" s="140"/>
-      <c r="U14" s="144" t="s">
+      <c r="T14" s="125"/>
+      <c r="U14" s="125"/>
+      <c r="V14" s="142" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="145" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="141" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="129" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="126" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="141" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="141" t="s">
+      <c r="C15" s="126" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="126" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="141" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="146" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="141" t="s">
+      <c r="F15" s="126" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="130" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="126" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="141" t="s">
-        <v>9</v>
-      </c>
-      <c r="I15" s="147" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="141" t="s">
+      <c r="I15" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="131" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="126" t="s">
         <v>96</v>
       </c>
-      <c r="K15" s="141" t="s">
-        <v>9</v>
-      </c>
-      <c r="L15" s="147" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15" s="141" t="s">
+      <c r="L15" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="131" t="s">
+        <v>17</v>
+      </c>
+      <c r="N15" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="N15" s="141"/>
-      <c r="O15" s="141"/>
-      <c r="P15" s="141" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q15" s="141" t="s">
+      <c r="O15" s="126"/>
+      <c r="P15" s="126"/>
+      <c r="Q15" s="126" t="s">
+        <v>29</v>
+      </c>
+      <c r="R15" s="126" t="s">
         <v>53</v>
       </c>
-      <c r="R15" s="141" t="s">
+      <c r="S15" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="S15" s="141">
+      <c r="T15" s="126">
         <v>1</v>
       </c>
-      <c r="T15" s="141">
+      <c r="U15" s="126">
         <v>0.01</v>
       </c>
-      <c r="U15" s="148"/>
+      <c r="V15" s="143"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="149" t="s">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="150" t="s">
+      <c r="B16" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="150" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="150" t="s">
+      <c r="C16" s="133" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="133" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="150" t="s">
+      <c r="F16" s="133" t="s">
         <v>94</v>
       </c>
-      <c r="F16" s="151" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="150" t="s">
+      <c r="G16" s="134" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="133" t="s">
         <v>96</v>
       </c>
-      <c r="H16" s="150" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="152" t="s">
-        <v>17</v>
-      </c>
-      <c r="J16" s="150" t="s">
+      <c r="I16" s="133" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="135" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="133" t="s">
         <v>96</v>
       </c>
-      <c r="K16" s="150" t="s">
+      <c r="L16" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="L16" s="152" t="s">
-        <v>17</v>
-      </c>
-      <c r="M16" s="150" t="s">
+      <c r="M16" s="135" t="s">
+        <v>17</v>
+      </c>
+      <c r="N16" s="133" t="s">
         <v>47</v>
       </c>
-      <c r="N16" s="150"/>
-      <c r="O16" s="150"/>
-      <c r="P16" s="150" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q16" s="150" t="s">
+      <c r="O16" s="133"/>
+      <c r="P16" s="133"/>
+      <c r="Q16" s="133" t="s">
+        <v>29</v>
+      </c>
+      <c r="R16" s="133" t="s">
         <v>54</v>
       </c>
-      <c r="R16" s="150" t="s">
+      <c r="S16" s="133" t="s">
         <v>55</v>
       </c>
-      <c r="S16" s="150"/>
-      <c r="T16" s="150"/>
-      <c r="U16" s="153"/>
+      <c r="T16" s="133"/>
+      <c r="U16" s="133"/>
+      <c r="V16" s="144"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="67" t="s">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="68" t="s">
+      <c r="C17" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="69" t="s">
+      <c r="F17" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="70" t="s">
+      <c r="G17" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="68" t="s">
+      <c r="H17" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="H17" s="68" t="s">
+      <c r="I17" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="I17" s="84" t="s">
+      <c r="J17" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="J17" s="68" t="s">
+      <c r="K17" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="K17" s="68" t="s">
-        <v>9</v>
-      </c>
-      <c r="L17" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="M17" s="68" t="s">
+      <c r="L17" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="N17" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="N17" s="68"/>
-      <c r="O17" s="68"/>
-      <c r="P17" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q17" s="89" t="s">
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="R17" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="R17" s="68" t="s">
+      <c r="S17" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="S17" s="68"/>
-      <c r="T17" s="68"/>
-      <c r="U17" s="72" t="s">
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="160" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="69" t="s">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="69" t="s">
+      <c r="C18" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="74" t="s">
+      <c r="F18" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="69" t="s">
+      <c r="H18" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="H18" s="69" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="69" t="s">
+      <c r="I18" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="K18" s="69" t="s">
-        <v>9</v>
-      </c>
-      <c r="L18" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="M18" s="69" t="s">
+      <c r="L18" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="N18" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q18" s="76" t="s">
+      <c r="O18" s="57"/>
+      <c r="P18" s="57"/>
+      <c r="Q18" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="R18" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="R18" s="69" t="s">
+      <c r="S18" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="S18" s="69">
+      <c r="T18" s="57">
         <v>1</v>
       </c>
-      <c r="T18" s="76">
+      <c r="U18" s="63">
         <v>0.01</v>
       </c>
-      <c r="U18" s="77"/>
+      <c r="V18" s="161"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="78" t="s">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="79" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="79" t="s">
+      <c r="C19" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="79" t="s">
+      <c r="F19" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="80" t="s">
+      <c r="G19" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="79" t="s">
+      <c r="H19" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="H19" s="79" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="81" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="79" t="s">
+      <c r="I19" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="K19" s="79" t="s">
+      <c r="L19" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="L19" s="81" t="s">
-        <v>17</v>
-      </c>
-      <c r="M19" s="79" t="s">
+      <c r="M19" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="N19" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="N19" s="79"/>
-      <c r="O19" s="79"/>
-      <c r="P19" s="79" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q19" s="90" t="s">
+      <c r="O19" s="65"/>
+      <c r="P19" s="65"/>
+      <c r="Q19" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="R19" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="R19" s="79" t="s">
+      <c r="S19" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="S19" s="79"/>
-      <c r="T19" s="79"/>
-      <c r="U19" s="82"/>
+      <c r="T19" s="65"/>
+      <c r="U19" s="65"/>
+      <c r="V19" s="162"/>
     </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="91" t="s">
+    <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="92" t="s">
+      <c r="B20" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="92" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="92" t="s">
+      <c r="C20" s="77" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="93" t="s">
+      <c r="F20" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="94" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="92" t="s">
+      <c r="G20" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="H20" s="92" t="s">
+      <c r="I20" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="I20" s="95" t="s">
+      <c r="J20" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="J20" s="92" t="s">
+      <c r="K20" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="K20" s="92" t="s">
-        <v>9</v>
-      </c>
-      <c r="L20" s="96" t="s">
-        <v>17</v>
-      </c>
-      <c r="M20" s="92" t="s">
+      <c r="L20" s="77" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" s="81" t="s">
+        <v>17</v>
+      </c>
+      <c r="N20" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="N20" s="92"/>
-      <c r="O20" s="92"/>
-      <c r="P20" s="92" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q20" s="97" t="s">
+      <c r="O20" s="77"/>
+      <c r="P20" s="77"/>
+      <c r="Q20" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="R20" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="R20" s="92" t="s">
+      <c r="S20" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="S20" s="92"/>
-      <c r="T20" s="92"/>
-      <c r="U20" s="157" t="s">
+      <c r="T20" s="77"/>
+      <c r="U20" s="77"/>
+      <c r="V20" s="136" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="98" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="93" t="s">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="83" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="93" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="93" t="s">
+      <c r="C21" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="93" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="99" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="93" t="s">
+      <c r="F21" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="84" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="100" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" s="93" t="s">
+      <c r="I21" s="78" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="K21" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21" s="100" t="s">
-        <v>17</v>
-      </c>
-      <c r="M21" s="93" t="s">
+      <c r="L21" s="78" t="s">
+        <v>9</v>
+      </c>
+      <c r="M21" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="N21" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="N21" s="93"/>
-      <c r="O21" s="93"/>
-      <c r="P21" s="93" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q21" s="101" t="s">
+      <c r="O21" s="78"/>
+      <c r="P21" s="78"/>
+      <c r="Q21" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="R21" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="R21" s="93" t="s">
+      <c r="S21" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="S21" s="93">
+      <c r="T21" s="78">
         <v>1</v>
       </c>
-      <c r="T21" s="101">
+      <c r="U21" s="86">
         <v>0.01</v>
       </c>
-      <c r="U21" s="158"/>
+      <c r="V21" s="137"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="102" t="s">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="103" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="103" t="s">
+      <c r="C22" s="88" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="88" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="103" t="s">
+      <c r="F22" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="104" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" s="103" t="s">
+      <c r="G22" s="89" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="88" t="s">
         <v>74</v>
       </c>
-      <c r="H22" s="103" t="s">
-        <v>9</v>
-      </c>
-      <c r="I22" s="105" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" s="103" t="s">
+      <c r="I22" s="88" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="K22" s="103" t="s">
+      <c r="L22" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="L22" s="105" t="s">
-        <v>17</v>
-      </c>
-      <c r="M22" s="103" t="s">
+      <c r="M22" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="N22" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="N22" s="103"/>
-      <c r="O22" s="103" t="s">
+      <c r="O22" s="88"/>
+      <c r="P22" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="P22" s="103" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q22" s="106" t="s">
+      <c r="Q22" s="88" t="s">
+        <v>29</v>
+      </c>
+      <c r="R22" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="R22" s="103" t="s">
+      <c r="S22" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="S22" s="103"/>
-      <c r="T22" s="103"/>
-      <c r="U22" s="159"/>
+      <c r="T22" s="88"/>
+      <c r="U22" s="88"/>
+      <c r="V22" s="138"/>
     </row>
-    <row r="23" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="107" t="s">
+    <row r="23" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="108" t="s">
+      <c r="B23" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="108" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="108" t="s">
+      <c r="C23" s="93" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="109" t="s">
+      <c r="F23" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="110" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23" s="108" t="s">
+      <c r="G23" s="95" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="H23" s="108" t="s">
+      <c r="I23" s="93" t="s">
         <v>80</v>
       </c>
-      <c r="I23" s="111" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="108" t="s">
+      <c r="J23" s="96" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="K23" s="108" t="s">
-        <v>9</v>
-      </c>
-      <c r="L23" s="112" t="s">
-        <v>17</v>
-      </c>
-      <c r="M23" s="108" t="s">
+      <c r="L23" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" s="97" t="s">
+        <v>17</v>
+      </c>
+      <c r="N23" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="N23" s="108"/>
-      <c r="O23" s="108"/>
-      <c r="P23" s="108" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q23" s="113" t="s">
+      <c r="O23" s="93"/>
+      <c r="P23" s="93"/>
+      <c r="Q23" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="R23" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="R23" s="108" t="s">
+      <c r="S23" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="S23" s="108"/>
-      <c r="T23" s="108"/>
-      <c r="U23" s="154" t="s">
+      <c r="T23" s="93"/>
+      <c r="U23" s="93"/>
+      <c r="V23" s="139" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="114" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="109" t="s">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="109" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="109" t="s">
+      <c r="C24" s="94" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="94" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="109" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" s="115" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="109" t="s">
+      <c r="F24" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="100" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="H24" s="109" t="s">
-        <v>9</v>
-      </c>
-      <c r="I24" s="116" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="109" t="s">
+      <c r="I24" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="101" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="K24" s="109" t="s">
-        <v>9</v>
-      </c>
-      <c r="L24" s="116" t="s">
-        <v>17</v>
-      </c>
-      <c r="M24" s="109" t="s">
+      <c r="L24" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="M24" s="101" t="s">
+        <v>17</v>
+      </c>
+      <c r="N24" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="N24" s="109"/>
-      <c r="O24" s="109"/>
-      <c r="P24" s="109" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q24" s="117" t="s">
+      <c r="O24" s="94"/>
+      <c r="P24" s="94"/>
+      <c r="Q24" s="94" t="s">
+        <v>29</v>
+      </c>
+      <c r="R24" s="102" t="s">
         <v>54</v>
       </c>
-      <c r="R24" s="109" t="s">
+      <c r="S24" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="S24" s="109">
+      <c r="T24" s="94">
         <v>1</v>
       </c>
-      <c r="T24" s="117">
+      <c r="U24" s="102">
         <v>0.01</v>
       </c>
-      <c r="U24" s="155"/>
+      <c r="V24" s="140"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="118" t="s">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="119" t="s">
+      <c r="B25" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="119" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="119" t="s">
+      <c r="C25" s="104" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="104" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="119" t="s">
+      <c r="F25" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="F25" s="120" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" s="119" t="s">
+      <c r="G25" s="105" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="H25" s="119" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" s="121" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25" s="119" t="s">
+      <c r="I25" s="104" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="106" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="K25" s="119" t="s">
+      <c r="L25" s="104" t="s">
         <v>80</v>
       </c>
-      <c r="L25" s="121" t="s">
-        <v>17</v>
-      </c>
-      <c r="M25" s="119" t="s">
+      <c r="M25" s="106" t="s">
+        <v>17</v>
+      </c>
+      <c r="N25" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="N25" s="119"/>
-      <c r="O25" s="119" t="s">
+      <c r="O25" s="104"/>
+      <c r="P25" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="P25" s="119" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q25" s="122" t="s">
+      <c r="Q25" s="104" t="s">
+        <v>29</v>
+      </c>
+      <c r="R25" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="R25" s="119" t="s">
+      <c r="S25" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="S25" s="119"/>
-      <c r="T25" s="119"/>
-      <c r="U25" s="156"/>
+      <c r="T25" s="104"/>
+      <c r="U25" s="104"/>
+      <c r="V25" s="141"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="123" t="s">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="124" t="s">
+      <c r="B26" s="109" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="124" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="124" t="s">
+      <c r="C26" s="109" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="109" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="125" t="s">
+      <c r="F26" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="F26" s="126" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="124" t="s">
+      <c r="G26" s="111" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="109" t="s">
         <v>88</v>
       </c>
-      <c r="H26" s="124" t="s">
+      <c r="I26" s="109" t="s">
         <v>80</v>
       </c>
-      <c r="I26" s="127" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="124" t="s">
+      <c r="J26" s="112" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26" s="109" t="s">
         <v>88</v>
       </c>
-      <c r="K26" s="124" t="s">
-        <v>9</v>
-      </c>
-      <c r="L26" s="128" t="s">
-        <v>17</v>
-      </c>
-      <c r="M26" s="124" t="s">
+      <c r="L26" s="109" t="s">
+        <v>9</v>
+      </c>
+      <c r="M26" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="N26" s="109" t="s">
         <v>69</v>
       </c>
-      <c r="N26" s="124"/>
-      <c r="O26" s="124"/>
-      <c r="P26" s="124" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q26" s="129" t="s">
+      <c r="O26" s="109"/>
+      <c r="P26" s="109"/>
+      <c r="Q26" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="R26" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="R26" s="124" t="s">
+      <c r="S26" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="S26" s="124"/>
-      <c r="T26" s="124"/>
-      <c r="U26" s="160" t="s">
+      <c r="T26" s="109"/>
+      <c r="U26" s="109"/>
+      <c r="V26" s="145" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="130" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" s="125" t="s">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="115" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="125" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="125" t="s">
+      <c r="C27" s="110" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="110" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="125" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="131" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="125" t="s">
+      <c r="F27" s="110" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="116" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="110" t="s">
         <v>88</v>
       </c>
-      <c r="H27" s="125" t="s">
-        <v>9</v>
-      </c>
-      <c r="I27" s="132" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="125" t="s">
+      <c r="I27" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="117" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" s="110" t="s">
         <v>88</v>
       </c>
-      <c r="K27" s="125" t="s">
-        <v>9</v>
-      </c>
-      <c r="L27" s="132" t="s">
-        <v>17</v>
-      </c>
-      <c r="M27" s="125" t="s">
+      <c r="L27" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="M27" s="117" t="s">
+        <v>17</v>
+      </c>
+      <c r="N27" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="N27" s="125"/>
-      <c r="O27" s="125"/>
-      <c r="P27" s="125" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q27" s="133" t="s">
+      <c r="O27" s="110"/>
+      <c r="P27" s="110"/>
+      <c r="Q27" s="110" t="s">
+        <v>29</v>
+      </c>
+      <c r="R27" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="R27" s="125" t="s">
+      <c r="S27" s="110" t="s">
         <v>77</v>
       </c>
-      <c r="S27" s="125">
+      <c r="T27" s="110">
         <v>1</v>
       </c>
-      <c r="T27" s="133">
+      <c r="U27" s="118">
         <v>0.01</v>
       </c>
-      <c r="U27" s="161"/>
+      <c r="V27" s="146"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="134" t="s">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="135" t="s">
+      <c r="B28" s="120" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="135" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="135" t="s">
+      <c r="C28" s="120" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="120" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="135" t="s">
+      <c r="F28" s="120" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="136" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" s="135" t="s">
+      <c r="G28" s="121" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="120" t="s">
         <v>88</v>
       </c>
-      <c r="H28" s="135" t="s">
-        <v>9</v>
-      </c>
-      <c r="I28" s="137" t="s">
-        <v>17</v>
-      </c>
-      <c r="J28" s="135" t="s">
+      <c r="I28" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="120" t="s">
         <v>88</v>
       </c>
-      <c r="K28" s="135" t="s">
+      <c r="L28" s="120" t="s">
         <v>80</v>
       </c>
-      <c r="L28" s="137" t="s">
-        <v>17</v>
-      </c>
-      <c r="M28" s="135" t="s">
+      <c r="M28" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="N28" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="N28" s="135"/>
-      <c r="O28" s="135" t="s">
+      <c r="O28" s="120"/>
+      <c r="P28" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="P28" s="135" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q28" s="138" t="s">
+      <c r="Q28" s="120" t="s">
+        <v>29</v>
+      </c>
+      <c r="R28" s="123" t="s">
         <v>52</v>
       </c>
-      <c r="R28" s="135" t="s">
+      <c r="S28" s="120" t="s">
         <v>77</v>
       </c>
-      <c r="S28" s="135"/>
-      <c r="T28" s="135"/>
-      <c r="U28" s="162"/>
+      <c r="T28" s="120"/>
+      <c r="U28" s="120"/>
+      <c r="V28" s="147"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="U20:U22"/>
-    <mergeCell ref="U23:U25"/>
-    <mergeCell ref="U14:U16"/>
-    <mergeCell ref="U26:U28"/>
-    <mergeCell ref="U11:U13"/>
-    <mergeCell ref="U8:U10"/>
-    <mergeCell ref="U5:U7"/>
-    <mergeCell ref="U2:U4"/>
-    <mergeCell ref="U17:U19"/>
+    <mergeCell ref="V8:V10"/>
+    <mergeCell ref="V5:V7"/>
+    <mergeCell ref="V2:V4"/>
+    <mergeCell ref="V17:V19"/>
+    <mergeCell ref="V20:V22"/>
+    <mergeCell ref="V23:V25"/>
+    <mergeCell ref="V14:V16"/>
+    <mergeCell ref="V26:V28"/>
+    <mergeCell ref="V11:V13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Small changes in storage setup
</commit_message>
<xml_diff>
--- a/scenario work/add_storage_tech/setup_storage.xlsx
+++ b/scenario work/add_storage_tech/setup_storage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\time_clustering\scenario work\add_storage_tech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A733A3-1923-4530-9837-B0AB051ACA3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F94AF8C-631D-4991-876B-5C206364B5B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="19935" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="19935" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="storage" sheetId="20" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="109">
   <si>
     <t>technology</t>
   </si>
@@ -352,6 +352,33 @@
   </si>
   <si>
     <t>M1</t>
+  </si>
+  <si>
+    <t>hydro_phs_dam,M1</t>
+  </si>
+  <si>
+    <t>hydro_lc_dam,M1</t>
+  </si>
+  <si>
+    <t>hydro_hc_dam,M1</t>
+  </si>
+  <si>
+    <t>dh_stor_tank,M1</t>
+  </si>
+  <si>
+    <t>rc_stor_tank,M1</t>
+  </si>
+  <si>
+    <t>h2_stor_tank,M1</t>
+  </si>
+  <si>
+    <t>elec_stor_bank,M1</t>
+  </si>
+  <si>
+    <t>flex_rc_bank,M1</t>
+  </si>
+  <si>
+    <t>flex_i_bank,M1</t>
   </si>
 </sst>
 </file>
@@ -711,6 +738,42 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -754,42 +817,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1097,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F56DBD-A483-468D-94AB-6D22FF1A0021}">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,7 +1133,7 @@
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" customWidth="1"/>
     <col min="4" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
@@ -1209,7 +1236,7 @@
         <v>31</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>4</v>
@@ -1248,7 +1275,7 @@
       </c>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
-      <c r="V2" s="157" t="s">
+      <c r="V2" s="142" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1312,7 +1339,7 @@
       <c r="U3" s="48">
         <v>0.01</v>
       </c>
-      <c r="V3" s="158"/>
+      <c r="V3" s="143"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1331,7 +1358,7 @@
         <v>31</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>4</v>
@@ -1372,7 +1399,7 @@
       </c>
       <c r="T4" s="9"/>
       <c r="U4" s="48"/>
-      <c r="V4" s="159"/>
+      <c r="V4" s="144"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -1391,7 +1418,7 @@
         <v>31</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>4</v>
@@ -1432,7 +1459,7 @@
       </c>
       <c r="T5" s="13"/>
       <c r="U5" s="49"/>
-      <c r="V5" s="154" t="s">
+      <c r="V5" s="139" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1498,7 +1525,7 @@
       <c r="U6" s="50">
         <v>0.01</v>
       </c>
-      <c r="V6" s="155"/>
+      <c r="V6" s="140"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
@@ -1517,7 +1544,7 @@
         <v>31</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="G7" s="22" t="s">
         <v>4</v>
@@ -1560,7 +1587,7 @@
       </c>
       <c r="T7" s="21"/>
       <c r="U7" s="51"/>
-      <c r="V7" s="156"/>
+      <c r="V7" s="141"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
@@ -1579,7 +1606,7 @@
         <v>31</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="G8" s="26" t="s">
         <v>4</v>
@@ -1620,7 +1647,7 @@
       </c>
       <c r="T8" s="25"/>
       <c r="U8" s="52"/>
-      <c r="V8" s="151" t="s">
+      <c r="V8" s="136" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1686,7 +1713,7 @@
       <c r="U9" s="53">
         <v>0.01</v>
       </c>
-      <c r="V9" s="152"/>
+      <c r="V9" s="137"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
@@ -1705,7 +1732,7 @@
         <v>31</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="G10" s="34" t="s">
         <v>4</v>
@@ -1748,7 +1775,7 @@
       </c>
       <c r="T10" s="33"/>
       <c r="U10" s="33"/>
-      <c r="V10" s="153"/>
+      <c r="V10" s="138"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
@@ -1767,7 +1794,7 @@
         <v>31</v>
       </c>
       <c r="F11" s="41" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="G11" s="38" t="s">
         <v>4</v>
@@ -1806,7 +1833,7 @@
       </c>
       <c r="T11" s="37"/>
       <c r="U11" s="37"/>
-      <c r="V11" s="148" t="s">
+      <c r="V11" s="160" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1870,7 +1897,7 @@
       <c r="U12" s="54">
         <v>0.01</v>
       </c>
-      <c r="V12" s="149"/>
+      <c r="V12" s="161"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
@@ -1889,7 +1916,7 @@
         <v>31</v>
       </c>
       <c r="F13" s="45" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="G13" s="46" t="s">
         <v>4</v>
@@ -1928,7 +1955,7 @@
       </c>
       <c r="T13" s="45"/>
       <c r="U13" s="45"/>
-      <c r="V13" s="150"/>
+      <c r="V13" s="162"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="124" t="s">
@@ -1947,7 +1974,7 @@
         <v>31</v>
       </c>
       <c r="F14" s="126" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="G14" s="127" t="s">
         <v>4</v>
@@ -1986,7 +2013,7 @@
       </c>
       <c r="T14" s="125"/>
       <c r="U14" s="125"/>
-      <c r="V14" s="142" t="s">
+      <c r="V14" s="154" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2050,7 +2077,7 @@
       <c r="U15" s="126">
         <v>0.01</v>
       </c>
-      <c r="V15" s="143"/>
+      <c r="V15" s="155"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="132" t="s">
@@ -2069,7 +2096,7 @@
         <v>31</v>
       </c>
       <c r="F16" s="133" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="G16" s="134" t="s">
         <v>4</v>
@@ -2108,7 +2135,7 @@
       </c>
       <c r="T16" s="133"/>
       <c r="U16" s="133"/>
-      <c r="V16" s="144"/>
+      <c r="V16" s="156"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
@@ -2127,7 +2154,7 @@
         <v>31</v>
       </c>
       <c r="F17" s="57" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="G17" s="58" t="s">
         <v>68</v>
@@ -2166,7 +2193,7 @@
       </c>
       <c r="T17" s="56"/>
       <c r="U17" s="56"/>
-      <c r="V17" s="160" t="s">
+      <c r="V17" s="145" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2230,7 +2257,7 @@
       <c r="U18" s="63">
         <v>0.01</v>
       </c>
-      <c r="V18" s="161"/>
+      <c r="V18" s="146"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="64" t="s">
@@ -2249,7 +2276,7 @@
         <v>31</v>
       </c>
       <c r="F19" s="65" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="G19" s="66" t="s">
         <v>68</v>
@@ -2288,7 +2315,7 @@
       </c>
       <c r="T19" s="65"/>
       <c r="U19" s="65"/>
-      <c r="V19" s="162"/>
+      <c r="V19" s="147"/>
     </row>
     <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="76" t="s">
@@ -2307,7 +2334,7 @@
         <v>31</v>
       </c>
       <c r="F20" s="78" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="G20" s="79" t="s">
         <v>4</v>
@@ -2346,7 +2373,7 @@
       </c>
       <c r="T20" s="77"/>
       <c r="U20" s="77"/>
-      <c r="V20" s="136" t="s">
+      <c r="V20" s="148" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2410,7 +2437,7 @@
       <c r="U21" s="86">
         <v>0.01</v>
       </c>
-      <c r="V21" s="137"/>
+      <c r="V21" s="149"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="87" t="s">
@@ -2429,7 +2456,7 @@
         <v>31</v>
       </c>
       <c r="F22" s="88" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="G22" s="89" t="s">
         <v>4</v>
@@ -2470,7 +2497,7 @@
       </c>
       <c r="T22" s="88"/>
       <c r="U22" s="88"/>
-      <c r="V22" s="138"/>
+      <c r="V22" s="150"/>
     </row>
     <row r="23" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="92" t="s">
@@ -2489,7 +2516,7 @@
         <v>31</v>
       </c>
       <c r="F23" s="94" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="G23" s="95" t="s">
         <v>4</v>
@@ -2528,7 +2555,7 @@
       </c>
       <c r="T23" s="93"/>
       <c r="U23" s="93"/>
-      <c r="V23" s="139" t="s">
+      <c r="V23" s="151" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2592,7 +2619,7 @@
       <c r="U24" s="102">
         <v>0.01</v>
       </c>
-      <c r="V24" s="140"/>
+      <c r="V24" s="152"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="103" t="s">
@@ -2611,7 +2638,7 @@
         <v>31</v>
       </c>
       <c r="F25" s="104" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="G25" s="105" t="s">
         <v>4</v>
@@ -2652,7 +2679,7 @@
       </c>
       <c r="T25" s="104"/>
       <c r="U25" s="104"/>
-      <c r="V25" s="141"/>
+      <c r="V25" s="153"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="108" t="s">
@@ -2671,7 +2698,7 @@
         <v>31</v>
       </c>
       <c r="F26" s="110" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="G26" s="111" t="s">
         <v>4</v>
@@ -2710,7 +2737,7 @@
       </c>
       <c r="T26" s="109"/>
       <c r="U26" s="109"/>
-      <c r="V26" s="145" t="s">
+      <c r="V26" s="157" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2774,7 +2801,7 @@
       <c r="U27" s="118">
         <v>0.01</v>
       </c>
-      <c r="V27" s="146"/>
+      <c r="V27" s="158"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="119" t="s">
@@ -2793,7 +2820,7 @@
         <v>31</v>
       </c>
       <c r="F28" s="120" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="G28" s="121" t="s">
         <v>4</v>
@@ -2834,19 +2861,19 @@
       </c>
       <c r="T28" s="120"/>
       <c r="U28" s="120"/>
-      <c r="V28" s="147"/>
+      <c r="V28" s="159"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="V23:V25"/>
+    <mergeCell ref="V14:V16"/>
+    <mergeCell ref="V26:V28"/>
+    <mergeCell ref="V11:V13"/>
     <mergeCell ref="V8:V10"/>
     <mergeCell ref="V5:V7"/>
     <mergeCell ref="V2:V4"/>
     <mergeCell ref="V17:V19"/>
     <mergeCell ref="V20:V22"/>
-    <mergeCell ref="V23:V25"/>
-    <mergeCell ref="V14:V16"/>
-    <mergeCell ref="V26:V28"/>
-    <mergeCell ref="V11:V13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add "lvl_temporal" to storage setup Excel file
</commit_message>
<xml_diff>
--- a/scenario work/add_storage_tech/setup_storage.xlsx
+++ b/scenario work/add_storage_tech/setup_storage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\time_clustering\scenario work\add_storage_tech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A733A3-1923-4530-9837-B0AB051ACA3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C31320-0D2F-4999-BBAA-734740BE441A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="19935" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="975" yWindow="1950" windowWidth="22065" windowHeight="8955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="storage" sheetId="20" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>tc={2A9BC780-3573-49FC-934D-EB88E44ABA62}</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{2A9BC780-3573-49FC-934D-EB88E44ABA62}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{2A9BC780-3573-49FC-934D-EB88E44ABA62}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="102">
   <si>
     <t>technology</t>
   </si>
@@ -352,6 +352,12 @@
   </si>
   <si>
     <t>M1</t>
+  </si>
+  <si>
+    <t>lvl_temporal</t>
+  </si>
+  <si>
+    <t>subannual</t>
   </si>
 </sst>
 </file>
@@ -711,6 +717,42 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -754,42 +796,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1087,7 +1093,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D1" dT="2019-11-26T17:01:21.48" personId="{5B2321EA-5DE5-468C-9F9C-016B7D7F0B1F}" id="{2A9BC780-3573-49FC-934D-EB88E44ABA62}">
+  <threadedComment ref="E1" dT="2019-11-26T17:01:21.48" personId="{5B2321EA-5DE5-468C-9F9C-016B7D7F0B1F}" id="{2A9BC780-3573-49FC-934D-EB88E44ABA62}">
     <text>either 'all' or one string or strings seprated by (/)</text>
   </threadedComment>
 </ThreadedComments>
@@ -1095,36 +1101,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F56DBD-A483-468D-94AB-6D22FF1A0021}">
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" customWidth="1"/>
-    <col min="4" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.85546875" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" customWidth="1"/>
-    <col min="22" max="22" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.85546875" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" customWidth="1"/>
+    <col min="23" max="23" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -1135,64 +1142,67 @@
         <v>98</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1202,57 +1212,58 @@
       <c r="C2" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="71" t="s">
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="T2" s="5"/>
       <c r="U2" s="5"/>
-      <c r="V2" s="157" t="s">
+      <c r="V2" s="5"/>
+      <c r="W2" s="142" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1263,58 +1274,61 @@
         <v>99</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="9" t="s">
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="9"/>
       <c r="P3" s="9"/>
-      <c r="Q3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" s="48" t="s">
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="T3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="9">
+      <c r="U3" s="9">
         <v>1</v>
       </c>
-      <c r="U3" s="48">
+      <c r="V3" s="48">
         <v>0.01</v>
       </c>
-      <c r="V3" s="158"/>
+      <c r="W3" s="143"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
@@ -1324,57 +1338,58 @@
       <c r="C4" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="N4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9" t="s">
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="Q4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" s="48" t="s">
+      <c r="R4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="T4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="T4" s="9"/>
-      <c r="U4" s="48"/>
-      <c r="V4" s="159"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="144"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
@@ -1384,59 +1399,60 @@
       <c r="C5" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="J5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>1</v>
+      <c r="M5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="O5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="R5" s="49" t="s">
+      <c r="P5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="T5" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="T5" s="13"/>
-      <c r="U5" s="49"/>
-      <c r="V5" s="154" t="s">
+      <c r="U5" s="13"/>
+      <c r="V5" s="49"/>
+      <c r="W5" s="139" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -1447,60 +1463,63 @@
         <v>99</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E6" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="17" t="s">
+      <c r="G6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="17" t="s">
+      <c r="J6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>1</v>
+      <c r="M6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="O6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="50" t="s">
+      <c r="P6" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="S6" s="17" t="s">
+      <c r="T6" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="T6" s="17">
+      <c r="U6" s="17">
         <v>1</v>
       </c>
-      <c r="U6" s="50">
+      <c r="V6" s="50">
         <v>0.01</v>
       </c>
-      <c r="V6" s="155"/>
+      <c r="W6" s="140"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>8</v>
       </c>
@@ -1510,38 +1529,36 @@
       <c r="C7" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="21" t="s">
-        <v>29</v>
-      </c>
+      <c r="D7" s="21"/>
       <c r="E7" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="G7" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="21" t="s">
+      <c r="J7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="M7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="N7" s="23" t="s">
         <v>28</v>
-      </c>
-      <c r="N7" s="21" t="s">
-        <v>1</v>
       </c>
       <c r="O7" s="21" t="s">
         <v>1</v>
@@ -1550,19 +1567,22 @@
         <v>1</v>
       </c>
       <c r="Q7" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="S7" s="21" t="s">
+      <c r="T7" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="T7" s="21"/>
-      <c r="U7" s="51"/>
-      <c r="V7" s="156"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="51"/>
+      <c r="W7" s="141"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>7</v>
       </c>
@@ -1572,59 +1592,60 @@
       <c r="C8" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>29</v>
-      </c>
+      <c r="D8" s="25"/>
       <c r="E8" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="G8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="J8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="N8" s="25" t="s">
-        <v>43</v>
+      <c r="M8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" s="27" t="s">
+        <v>17</v>
       </c>
       <c r="O8" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="R8" s="52" t="s">
+      <c r="P8" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="S8" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="S8" s="25" t="s">
+      <c r="T8" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="T8" s="25"/>
-      <c r="U8" s="52"/>
-      <c r="V8" s="151" t="s">
+      <c r="U8" s="25"/>
+      <c r="V8" s="52"/>
+      <c r="W8" s="136" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>9</v>
       </c>
@@ -1635,60 +1656,63 @@
         <v>99</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E9" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="29" t="s">
+      <c r="G9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="29" t="s">
+      <c r="J9" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="29" t="s">
-        <v>43</v>
+      <c r="M9" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="O9" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="R9" s="53" t="s">
+      <c r="P9" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="S9" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="S9" s="29" t="s">
+      <c r="T9" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="T9" s="29">
+      <c r="U9" s="29">
         <v>1</v>
       </c>
-      <c r="U9" s="53">
+      <c r="V9" s="53">
         <v>0.01</v>
       </c>
-      <c r="V9" s="152"/>
+      <c r="W9" s="137"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>8</v>
       </c>
@@ -1698,38 +1722,36 @@
       <c r="C10" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="33" t="s">
-        <v>29</v>
-      </c>
+      <c r="D10" s="33"/>
       <c r="E10" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="G10" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="33" t="s">
+      <c r="H10" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="33" t="s">
+      <c r="J10" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="33" t="s">
+      <c r="M10" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="35" t="s">
+      <c r="N10" s="35" t="s">
         <v>28</v>
-      </c>
-      <c r="N10" s="33" t="s">
-        <v>43</v>
       </c>
       <c r="O10" s="33" t="s">
         <v>43</v>
@@ -1738,19 +1760,22 @@
         <v>43</v>
       </c>
       <c r="Q10" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="R10" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="R10" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="S10" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="S10" s="33" t="s">
+      <c r="T10" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="T10" s="33"/>
       <c r="U10" s="33"/>
-      <c r="V10" s="153"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="138"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>7</v>
       </c>
@@ -1760,57 +1785,58 @@
       <c r="C11" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="37" t="s">
-        <v>29</v>
-      </c>
+      <c r="D11" s="37"/>
       <c r="E11" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="41" t="s">
+      <c r="G11" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="G11" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="37" t="s">
+      <c r="H11" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="37" t="s">
+      <c r="J11" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="68" t="s">
+      <c r="K11" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="37" t="s">
+      <c r="L11" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="M11" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="N11" s="37" t="s">
+      <c r="M11" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="O11" s="37"/>
       <c r="P11" s="37"/>
-      <c r="Q11" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="R11" s="73" t="s">
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="S11" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="S11" s="37" t="s">
+      <c r="T11" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="T11" s="37"/>
       <c r="U11" s="37"/>
-      <c r="V11" s="148" t="s">
+      <c r="V11" s="37"/>
+      <c r="W11" s="160" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>9</v>
       </c>
@@ -1821,58 +1847,61 @@
         <v>99</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E12" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="41" t="s">
+      <c r="G12" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="41" t="s">
+      <c r="J12" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="L12" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="M12" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="N12" s="41" t="s">
+      <c r="M12" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="O12" s="41"/>
       <c r="P12" s="41"/>
-      <c r="Q12" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="R12" s="54" t="s">
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="S12" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="S12" s="41" t="s">
+      <c r="T12" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="T12" s="41">
+      <c r="U12" s="41">
         <v>1</v>
       </c>
-      <c r="U12" s="54">
+      <c r="V12" s="54">
         <v>0.01</v>
       </c>
-      <c r="V12" s="149"/>
+      <c r="W12" s="161"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
         <v>8</v>
       </c>
@@ -1882,55 +1911,56 @@
       <c r="C13" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="45" t="s">
-        <v>29</v>
-      </c>
+      <c r="D13" s="45"/>
       <c r="E13" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="45" t="s">
+      <c r="G13" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="45" t="s">
+      <c r="H13" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="I13" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="45" t="s">
+      <c r="J13" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="L13" s="45" t="s">
+      <c r="M13" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="N13" s="45" t="s">
+      <c r="N13" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="O13" s="45"/>
       <c r="P13" s="45"/>
-      <c r="Q13" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="R13" s="70" t="s">
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="S13" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="S13" s="45" t="s">
+      <c r="T13" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="T13" s="45"/>
       <c r="U13" s="45"/>
-      <c r="V13" s="150"/>
+      <c r="V13" s="45"/>
+      <c r="W13" s="162"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="124" t="s">
         <v>7</v>
       </c>
@@ -1940,57 +1970,58 @@
       <c r="C14" s="125" t="s">
         <v>99</v>
       </c>
-      <c r="D14" s="125" t="s">
-        <v>29</v>
-      </c>
+      <c r="D14" s="125"/>
       <c r="E14" s="125" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="126" t="s">
+      <c r="G14" s="126" t="s">
         <v>94</v>
       </c>
-      <c r="G14" s="127" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="125" t="s">
+      <c r="H14" s="127" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="I14" s="125" t="s">
+      <c r="J14" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="128" t="s">
+      <c r="K14" s="128" t="s">
         <v>46</v>
       </c>
-      <c r="K14" s="125" t="s">
+      <c r="L14" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="L14" s="125" t="s">
-        <v>9</v>
-      </c>
-      <c r="M14" s="128" t="s">
-        <v>17</v>
-      </c>
-      <c r="N14" s="125" t="s">
+      <c r="M14" s="125" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="128" t="s">
+        <v>17</v>
+      </c>
+      <c r="O14" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="O14" s="125"/>
       <c r="P14" s="125"/>
-      <c r="Q14" s="125" t="s">
-        <v>29</v>
-      </c>
+      <c r="Q14" s="125"/>
       <c r="R14" s="125" t="s">
+        <v>29</v>
+      </c>
+      <c r="S14" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="S14" s="125" t="s">
+      <c r="T14" s="125" t="s">
         <v>55</v>
       </c>
-      <c r="T14" s="125"/>
       <c r="U14" s="125"/>
-      <c r="V14" s="142" t="s">
+      <c r="V14" s="125"/>
+      <c r="W14" s="154" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="129" t="s">
         <v>9</v>
       </c>
@@ -2001,58 +2032,61 @@
         <v>99</v>
       </c>
       <c r="D15" s="126" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E15" s="126" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="126" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="130" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="126" t="s">
+      <c r="G15" s="126" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="130" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="126" t="s">
         <v>96</v>
       </c>
-      <c r="I15" s="126" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="131" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15" s="126" t="s">
+      <c r="J15" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="131" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="126" t="s">
         <v>96</v>
       </c>
-      <c r="L15" s="126" t="s">
-        <v>9</v>
-      </c>
-      <c r="M15" s="131" t="s">
-        <v>17</v>
-      </c>
-      <c r="N15" s="126" t="s">
+      <c r="M15" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" s="131" t="s">
+        <v>17</v>
+      </c>
+      <c r="O15" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="O15" s="126"/>
       <c r="P15" s="126"/>
-      <c r="Q15" s="126" t="s">
-        <v>29</v>
-      </c>
+      <c r="Q15" s="126"/>
       <c r="R15" s="126" t="s">
+        <v>29</v>
+      </c>
+      <c r="S15" s="126" t="s">
         <v>53</v>
       </c>
-      <c r="S15" s="126" t="s">
+      <c r="T15" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="T15" s="126">
+      <c r="U15" s="126">
         <v>1</v>
       </c>
-      <c r="U15" s="126">
+      <c r="V15" s="126">
         <v>0.01</v>
       </c>
-      <c r="V15" s="143"/>
+      <c r="W15" s="155"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="132" t="s">
         <v>8</v>
       </c>
@@ -2062,55 +2096,56 @@
       <c r="C16" s="133" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="133" t="s">
-        <v>29</v>
-      </c>
+      <c r="D16" s="133"/>
       <c r="E16" s="133" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="133" t="s">
+      <c r="G16" s="133" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="134" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="133" t="s">
+      <c r="H16" s="134" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="133" t="s">
         <v>96</v>
       </c>
-      <c r="I16" s="133" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="135" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="133" t="s">
+      <c r="J16" s="133" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="135" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="133" t="s">
         <v>96</v>
       </c>
-      <c r="L16" s="133" t="s">
+      <c r="M16" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="M16" s="135" t="s">
-        <v>17</v>
-      </c>
-      <c r="N16" s="133" t="s">
+      <c r="N16" s="135" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16" s="133" t="s">
         <v>47</v>
       </c>
-      <c r="O16" s="133"/>
       <c r="P16" s="133"/>
-      <c r="Q16" s="133" t="s">
-        <v>29</v>
-      </c>
+      <c r="Q16" s="133"/>
       <c r="R16" s="133" t="s">
+        <v>29</v>
+      </c>
+      <c r="S16" s="133" t="s">
         <v>54</v>
       </c>
-      <c r="S16" s="133" t="s">
+      <c r="T16" s="133" t="s">
         <v>55</v>
       </c>
-      <c r="T16" s="133"/>
       <c r="U16" s="133"/>
-      <c r="V16" s="144"/>
+      <c r="V16" s="133"/>
+      <c r="W16" s="156"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
         <v>7</v>
       </c>
@@ -2120,57 +2155,58 @@
       <c r="C17" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="56" t="s">
-        <v>29</v>
-      </c>
+      <c r="D17" s="56"/>
       <c r="E17" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="57" t="s">
+      <c r="G17" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="58" t="s">
+      <c r="H17" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="H17" s="56" t="s">
+      <c r="I17" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="I17" s="56" t="s">
+      <c r="J17" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="J17" s="69" t="s">
+      <c r="K17" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="K17" s="56" t="s">
+      <c r="L17" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="L17" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="M17" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="N17" s="56" t="s">
+      <c r="M17" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="O17" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="O17" s="56"/>
       <c r="P17" s="56"/>
-      <c r="Q17" s="56" t="s">
-        <v>29</v>
-      </c>
-      <c r="R17" s="74" t="s">
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="S17" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="S17" s="56" t="s">
+      <c r="T17" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="T17" s="56"/>
       <c r="U17" s="56"/>
-      <c r="V17" s="160" t="s">
+      <c r="V17" s="56"/>
+      <c r="W17" s="145" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="s">
         <v>9</v>
       </c>
@@ -2181,58 +2217,61 @@
         <v>99</v>
       </c>
       <c r="D18" s="57" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E18" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="61" t="s">
+      <c r="G18" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="57" t="s">
+      <c r="I18" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="I18" s="57" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="57" t="s">
+      <c r="J18" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="L18" s="57" t="s">
-        <v>9</v>
-      </c>
-      <c r="M18" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="N18" s="57" t="s">
+      <c r="M18" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="O18" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="O18" s="57"/>
       <c r="P18" s="57"/>
-      <c r="Q18" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="R18" s="63" t="s">
+      <c r="Q18" s="57"/>
+      <c r="R18" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="S18" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="S18" s="57" t="s">
+      <c r="T18" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="T18" s="57">
+      <c r="U18" s="57">
         <v>1</v>
       </c>
-      <c r="U18" s="63">
+      <c r="V18" s="63">
         <v>0.01</v>
       </c>
-      <c r="V18" s="161"/>
+      <c r="W18" s="146"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="64" t="s">
         <v>8</v>
       </c>
@@ -2242,55 +2281,56 @@
       <c r="C19" s="65" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="65" t="s">
-        <v>29</v>
-      </c>
+      <c r="D19" s="65"/>
       <c r="E19" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="65" t="s">
+      <c r="G19" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="66" t="s">
+      <c r="H19" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="H19" s="65" t="s">
+      <c r="I19" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="I19" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" s="65" t="s">
+      <c r="J19" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="L19" s="65" t="s">
+      <c r="M19" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="M19" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="N19" s="65" t="s">
+      <c r="N19" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="O19" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="O19" s="65"/>
       <c r="P19" s="65"/>
-      <c r="Q19" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="R19" s="75" t="s">
+      <c r="Q19" s="65"/>
+      <c r="R19" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="S19" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="S19" s="65" t="s">
+      <c r="T19" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="T19" s="65"/>
       <c r="U19" s="65"/>
-      <c r="V19" s="162"/>
+      <c r="V19" s="65"/>
+      <c r="W19" s="147"/>
     </row>
-    <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="76" t="s">
         <v>7</v>
       </c>
@@ -2300,57 +2340,58 @@
       <c r="C20" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="77" t="s">
-        <v>29</v>
-      </c>
+      <c r="D20" s="77"/>
       <c r="E20" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="78" t="s">
+      <c r="G20" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="77" t="s">
+      <c r="H20" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="I20" s="77" t="s">
+      <c r="J20" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="80" t="s">
+      <c r="K20" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="K20" s="77" t="s">
+      <c r="L20" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="L20" s="77" t="s">
-        <v>9</v>
-      </c>
-      <c r="M20" s="81" t="s">
-        <v>17</v>
-      </c>
-      <c r="N20" s="77" t="s">
+      <c r="M20" s="77" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" s="81" t="s">
+        <v>17</v>
+      </c>
+      <c r="O20" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="O20" s="77"/>
       <c r="P20" s="77"/>
-      <c r="Q20" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="R20" s="82" t="s">
+      <c r="Q20" s="77"/>
+      <c r="R20" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="S20" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="S20" s="77" t="s">
+      <c r="T20" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="T20" s="77"/>
       <c r="U20" s="77"/>
-      <c r="V20" s="136" t="s">
+      <c r="V20" s="77"/>
+      <c r="W20" s="148" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="83" t="s">
         <v>9</v>
       </c>
@@ -2361,58 +2402,61 @@
         <v>99</v>
       </c>
       <c r="D21" s="78" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E21" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="84" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="78" t="s">
+      <c r="G21" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="84" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="I21" s="78" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" s="85" t="s">
-        <v>17</v>
-      </c>
-      <c r="K21" s="78" t="s">
+      <c r="J21" s="78" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="L21" s="78" t="s">
-        <v>9</v>
-      </c>
-      <c r="M21" s="85" t="s">
-        <v>17</v>
-      </c>
-      <c r="N21" s="78" t="s">
+      <c r="M21" s="78" t="s">
+        <v>9</v>
+      </c>
+      <c r="N21" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="O21" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="O21" s="78"/>
       <c r="P21" s="78"/>
-      <c r="Q21" s="78" t="s">
-        <v>29</v>
-      </c>
-      <c r="R21" s="86" t="s">
+      <c r="Q21" s="78"/>
+      <c r="R21" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="S21" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="S21" s="78" t="s">
+      <c r="T21" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="T21" s="78">
+      <c r="U21" s="78">
         <v>1</v>
       </c>
-      <c r="U21" s="86">
+      <c r="V21" s="86">
         <v>0.01</v>
       </c>
-      <c r="V21" s="137"/>
+      <c r="W21" s="149"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="87" t="s">
         <v>8</v>
       </c>
@@ -2422,57 +2466,58 @@
       <c r="C22" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="88" t="s">
-        <v>29</v>
-      </c>
+      <c r="D22" s="88"/>
       <c r="E22" s="88" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="88" t="s">
+      <c r="G22" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="G22" s="89" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="88" t="s">
+      <c r="H22" s="89" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="88" t="s">
         <v>74</v>
       </c>
-      <c r="I22" s="88" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" s="90" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="88" t="s">
+      <c r="J22" s="88" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="L22" s="88" t="s">
+      <c r="M22" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="M22" s="90" t="s">
-        <v>17</v>
-      </c>
-      <c r="N22" s="88" t="s">
+      <c r="N22" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="O22" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="O22" s="88"/>
-      <c r="P22" s="88" t="s">
+      <c r="P22" s="88"/>
+      <c r="Q22" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="Q22" s="88" t="s">
-        <v>29</v>
-      </c>
-      <c r="R22" s="91" t="s">
+      <c r="R22" s="88" t="s">
+        <v>29</v>
+      </c>
+      <c r="S22" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="S22" s="88" t="s">
+      <c r="T22" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="T22" s="88"/>
       <c r="U22" s="88"/>
-      <c r="V22" s="138"/>
+      <c r="V22" s="88"/>
+      <c r="W22" s="150"/>
     </row>
-    <row r="23" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="92" t="s">
         <v>7</v>
       </c>
@@ -2482,57 +2527,58 @@
       <c r="C23" s="93" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="93" t="s">
-        <v>29</v>
-      </c>
+      <c r="D23" s="93"/>
       <c r="E23" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="94" t="s">
+      <c r="G23" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="G23" s="95" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" s="93" t="s">
+      <c r="H23" s="95" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="I23" s="93" t="s">
+      <c r="J23" s="93" t="s">
         <v>80</v>
       </c>
-      <c r="J23" s="96" t="s">
-        <v>17</v>
-      </c>
-      <c r="K23" s="93" t="s">
+      <c r="K23" s="96" t="s">
+        <v>17</v>
+      </c>
+      <c r="L23" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="L23" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="M23" s="97" t="s">
-        <v>17</v>
-      </c>
-      <c r="N23" s="93" t="s">
+      <c r="M23" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="N23" s="97" t="s">
+        <v>17</v>
+      </c>
+      <c r="O23" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="O23" s="93"/>
       <c r="P23" s="93"/>
-      <c r="Q23" s="93" t="s">
-        <v>29</v>
-      </c>
-      <c r="R23" s="98" t="s">
+      <c r="Q23" s="93"/>
+      <c r="R23" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="S23" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="S23" s="93" t="s">
+      <c r="T23" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="T23" s="93"/>
       <c r="U23" s="93"/>
-      <c r="V23" s="139" t="s">
+      <c r="V23" s="93"/>
+      <c r="W23" s="151" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="99" t="s">
         <v>9</v>
       </c>
@@ -2543,58 +2589,61 @@
         <v>99</v>
       </c>
       <c r="D24" s="94" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E24" s="94" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="94" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="100" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" s="94" t="s">
+      <c r="G24" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="100" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="I24" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="J24" s="101" t="s">
-        <v>17</v>
-      </c>
-      <c r="K24" s="94" t="s">
+      <c r="J24" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="K24" s="101" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="L24" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="M24" s="101" t="s">
-        <v>17</v>
-      </c>
-      <c r="N24" s="94" t="s">
+      <c r="M24" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="N24" s="101" t="s">
+        <v>17</v>
+      </c>
+      <c r="O24" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="O24" s="94"/>
       <c r="P24" s="94"/>
-      <c r="Q24" s="94" t="s">
-        <v>29</v>
-      </c>
-      <c r="R24" s="102" t="s">
+      <c r="Q24" s="94"/>
+      <c r="R24" s="94" t="s">
+        <v>29</v>
+      </c>
+      <c r="S24" s="102" t="s">
         <v>54</v>
       </c>
-      <c r="S24" s="94" t="s">
+      <c r="T24" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="T24" s="94">
+      <c r="U24" s="94">
         <v>1</v>
       </c>
-      <c r="U24" s="102">
+      <c r="V24" s="102">
         <v>0.01</v>
       </c>
-      <c r="V24" s="140"/>
+      <c r="W24" s="152"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="103" t="s">
         <v>8</v>
       </c>
@@ -2604,57 +2653,58 @@
       <c r="C25" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="104" t="s">
-        <v>29</v>
-      </c>
+      <c r="D25" s="104"/>
       <c r="E25" s="104" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="104" t="s">
+      <c r="G25" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="G25" s="105" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" s="104" t="s">
+      <c r="H25" s="105" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="I25" s="104" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25" s="106" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" s="104" t="s">
+      <c r="J25" s="104" t="s">
+        <v>9</v>
+      </c>
+      <c r="K25" s="106" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="L25" s="104" t="s">
+      <c r="M25" s="104" t="s">
         <v>80</v>
       </c>
-      <c r="M25" s="106" t="s">
-        <v>17</v>
-      </c>
-      <c r="N25" s="104" t="s">
+      <c r="N25" s="106" t="s">
+        <v>17</v>
+      </c>
+      <c r="O25" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="O25" s="104"/>
-      <c r="P25" s="104" t="s">
+      <c r="P25" s="104"/>
+      <c r="Q25" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="Q25" s="104" t="s">
-        <v>29</v>
-      </c>
-      <c r="R25" s="107" t="s">
+      <c r="R25" s="104" t="s">
+        <v>29</v>
+      </c>
+      <c r="S25" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="S25" s="104" t="s">
+      <c r="T25" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="T25" s="104"/>
       <c r="U25" s="104"/>
-      <c r="V25" s="141"/>
+      <c r="V25" s="104"/>
+      <c r="W25" s="153"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="108" t="s">
         <v>7</v>
       </c>
@@ -2664,57 +2714,58 @@
       <c r="C26" s="109" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="109" t="s">
-        <v>29</v>
-      </c>
+      <c r="D26" s="109"/>
       <c r="E26" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="109" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="110" t="s">
+      <c r="G26" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="G26" s="111" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="109" t="s">
+      <c r="H26" s="111" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="109" t="s">
         <v>88</v>
       </c>
-      <c r="I26" s="109" t="s">
+      <c r="J26" s="109" t="s">
         <v>80</v>
       </c>
-      <c r="J26" s="112" t="s">
-        <v>17</v>
-      </c>
-      <c r="K26" s="109" t="s">
+      <c r="K26" s="112" t="s">
+        <v>17</v>
+      </c>
+      <c r="L26" s="109" t="s">
         <v>88</v>
       </c>
-      <c r="L26" s="109" t="s">
-        <v>9</v>
-      </c>
-      <c r="M26" s="113" t="s">
-        <v>17</v>
-      </c>
-      <c r="N26" s="109" t="s">
+      <c r="M26" s="109" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="O26" s="109" t="s">
         <v>69</v>
       </c>
-      <c r="O26" s="109"/>
       <c r="P26" s="109"/>
-      <c r="Q26" s="109" t="s">
-        <v>29</v>
-      </c>
-      <c r="R26" s="114" t="s">
+      <c r="Q26" s="109"/>
+      <c r="R26" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="S26" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="S26" s="109" t="s">
+      <c r="T26" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="T26" s="109"/>
       <c r="U26" s="109"/>
-      <c r="V26" s="145" t="s">
+      <c r="V26" s="109"/>
+      <c r="W26" s="157" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="115" t="s">
         <v>9</v>
       </c>
@@ -2725,58 +2776,61 @@
         <v>99</v>
       </c>
       <c r="D27" s="110" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E27" s="110" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="110" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="116" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="110" t="s">
+      <c r="G27" s="110" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="116" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="110" t="s">
         <v>88</v>
       </c>
-      <c r="I27" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="J27" s="117" t="s">
-        <v>17</v>
-      </c>
-      <c r="K27" s="110" t="s">
+      <c r="J27" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="K27" s="117" t="s">
+        <v>17</v>
+      </c>
+      <c r="L27" s="110" t="s">
         <v>88</v>
       </c>
-      <c r="L27" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="M27" s="117" t="s">
-        <v>17</v>
-      </c>
-      <c r="N27" s="110" t="s">
+      <c r="M27" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="N27" s="117" t="s">
+        <v>17</v>
+      </c>
+      <c r="O27" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="O27" s="110"/>
       <c r="P27" s="110"/>
-      <c r="Q27" s="110" t="s">
-        <v>29</v>
-      </c>
-      <c r="R27" s="118" t="s">
+      <c r="Q27" s="110"/>
+      <c r="R27" s="110" t="s">
+        <v>29</v>
+      </c>
+      <c r="S27" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="S27" s="110" t="s">
+      <c r="T27" s="110" t="s">
         <v>77</v>
       </c>
-      <c r="T27" s="110">
+      <c r="U27" s="110">
         <v>1</v>
       </c>
-      <c r="U27" s="118">
+      <c r="V27" s="118">
         <v>0.01</v>
       </c>
-      <c r="V27" s="146"/>
+      <c r="W27" s="158"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="119" t="s">
         <v>8</v>
       </c>
@@ -2786,67 +2840,68 @@
       <c r="C28" s="120" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="120" t="s">
-        <v>29</v>
-      </c>
+      <c r="D28" s="120"/>
       <c r="E28" s="120" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="120" t="s">
+      <c r="G28" s="120" t="s">
         <v>86</v>
       </c>
-      <c r="G28" s="121" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="120" t="s">
+      <c r="H28" s="121" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="120" t="s">
         <v>88</v>
       </c>
-      <c r="I28" s="120" t="s">
-        <v>9</v>
-      </c>
-      <c r="J28" s="122" t="s">
-        <v>17</v>
-      </c>
-      <c r="K28" s="120" t="s">
+      <c r="J28" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="K28" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="120" t="s">
         <v>88</v>
       </c>
-      <c r="L28" s="120" t="s">
+      <c r="M28" s="120" t="s">
         <v>80</v>
       </c>
-      <c r="M28" s="122" t="s">
-        <v>17</v>
-      </c>
-      <c r="N28" s="120" t="s">
+      <c r="N28" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="O28" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="O28" s="120"/>
-      <c r="P28" s="120" t="s">
+      <c r="P28" s="120"/>
+      <c r="Q28" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="Q28" s="120" t="s">
-        <v>29</v>
-      </c>
-      <c r="R28" s="123" t="s">
+      <c r="R28" s="120" t="s">
+        <v>29</v>
+      </c>
+      <c r="S28" s="123" t="s">
         <v>52</v>
       </c>
-      <c r="S28" s="120" t="s">
+      <c r="T28" s="120" t="s">
         <v>77</v>
       </c>
-      <c r="T28" s="120"/>
       <c r="U28" s="120"/>
-      <c r="V28" s="147"/>
+      <c r="V28" s="120"/>
+      <c r="W28" s="159"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="V8:V10"/>
-    <mergeCell ref="V5:V7"/>
-    <mergeCell ref="V2:V4"/>
-    <mergeCell ref="V17:V19"/>
-    <mergeCell ref="V20:V22"/>
-    <mergeCell ref="V23:V25"/>
-    <mergeCell ref="V14:V16"/>
-    <mergeCell ref="V26:V28"/>
-    <mergeCell ref="V11:V13"/>
+    <mergeCell ref="W23:W25"/>
+    <mergeCell ref="W14:W16"/>
+    <mergeCell ref="W26:W28"/>
+    <mergeCell ref="W11:W13"/>
+    <mergeCell ref="W8:W10"/>
+    <mergeCell ref="W5:W7"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="W17:W19"/>
+    <mergeCell ref="W20:W22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Excel setup file for lvl_temporal
</commit_message>
<xml_diff>
--- a/scenario work/add_storage_tech/setup_storage.xlsx
+++ b/scenario work/add_storage_tech/setup_storage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\time_clustering\scenario work\add_storage_tech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F94AF8C-631D-4991-876B-5C206364B5B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C31320-0D2F-4999-BBAA-734740BE441A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="19935" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="975" yWindow="1950" windowWidth="22065" windowHeight="8955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="storage" sheetId="20" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>tc={2A9BC780-3573-49FC-934D-EB88E44ABA62}</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{2A9BC780-3573-49FC-934D-EB88E44ABA62}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{2A9BC780-3573-49FC-934D-EB88E44ABA62}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="102">
   <si>
     <t>technology</t>
   </si>
@@ -354,31 +354,10 @@
     <t>M1</t>
   </si>
   <si>
-    <t>hydro_phs_dam,M1</t>
-  </si>
-  <si>
-    <t>hydro_lc_dam,M1</t>
-  </si>
-  <si>
-    <t>hydro_hc_dam,M1</t>
-  </si>
-  <si>
-    <t>dh_stor_tank,M1</t>
-  </si>
-  <si>
-    <t>rc_stor_tank,M1</t>
-  </si>
-  <si>
-    <t>h2_stor_tank,M1</t>
-  </si>
-  <si>
-    <t>elec_stor_bank,M1</t>
-  </si>
-  <si>
-    <t>flex_rc_bank,M1</t>
-  </si>
-  <si>
-    <t>flex_i_bank,M1</t>
+    <t>lvl_temporal</t>
+  </si>
+  <si>
+    <t>subannual</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1093,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D1" dT="2019-11-26T17:01:21.48" personId="{5B2321EA-5DE5-468C-9F9C-016B7D7F0B1F}" id="{2A9BC780-3573-49FC-934D-EB88E44ABA62}">
+  <threadedComment ref="E1" dT="2019-11-26T17:01:21.48" personId="{5B2321EA-5DE5-468C-9F9C-016B7D7F0B1F}" id="{2A9BC780-3573-49FC-934D-EB88E44ABA62}">
     <text>either 'all' or one string or strings seprated by (/)</text>
   </threadedComment>
 </ThreadedComments>
@@ -1122,36 +1101,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F56DBD-A483-468D-94AB-6D22FF1A0021}">
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" customWidth="1"/>
-    <col min="4" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.85546875" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" customWidth="1"/>
-    <col min="22" max="22" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.85546875" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" customWidth="1"/>
+    <col min="23" max="23" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -1162,64 +1142,67 @@
         <v>98</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1229,57 +1212,58 @@
       <c r="C2" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="71" t="s">
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="T2" s="5"/>
       <c r="U2" s="5"/>
-      <c r="V2" s="142" t="s">
+      <c r="V2" s="5"/>
+      <c r="W2" s="142" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1290,58 +1274,61 @@
         <v>99</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="9" t="s">
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="9"/>
       <c r="P3" s="9"/>
-      <c r="Q3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" s="48" t="s">
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="T3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="9">
+      <c r="U3" s="9">
         <v>1</v>
       </c>
-      <c r="U3" s="48">
+      <c r="V3" s="48">
         <v>0.01</v>
       </c>
-      <c r="V3" s="143"/>
+      <c r="W3" s="143"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
@@ -1351,57 +1338,58 @@
       <c r="C4" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="G4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="N4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9" t="s">
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="Q4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" s="48" t="s">
+      <c r="R4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="T4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="T4" s="9"/>
-      <c r="U4" s="48"/>
-      <c r="V4" s="144"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="144"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
@@ -1411,59 +1399,60 @@
       <c r="C5" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="13" t="s">
+      <c r="G5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="J5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>1</v>
+      <c r="M5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="O5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="R5" s="49" t="s">
+      <c r="P5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="T5" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="T5" s="13"/>
-      <c r="U5" s="49"/>
-      <c r="V5" s="139" t="s">
+      <c r="U5" s="13"/>
+      <c r="V5" s="49"/>
+      <c r="W5" s="139" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -1474,60 +1463,63 @@
         <v>99</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E6" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="17" t="s">
+      <c r="G6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="17" t="s">
+      <c r="J6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>1</v>
+      <c r="M6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="O6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="50" t="s">
+      <c r="P6" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="S6" s="17" t="s">
+      <c r="T6" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="T6" s="17">
+      <c r="U6" s="17">
         <v>1</v>
       </c>
-      <c r="U6" s="50">
+      <c r="V6" s="50">
         <v>0.01</v>
       </c>
-      <c r="V6" s="140"/>
+      <c r="W6" s="140"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>8</v>
       </c>
@@ -1537,38 +1529,36 @@
       <c r="C7" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="21" t="s">
-        <v>29</v>
-      </c>
+      <c r="D7" s="21"/>
       <c r="E7" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="21" t="s">
+      <c r="G7" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="21" t="s">
+      <c r="J7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="M7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="N7" s="23" t="s">
         <v>28</v>
-      </c>
-      <c r="N7" s="21" t="s">
-        <v>1</v>
       </c>
       <c r="O7" s="21" t="s">
         <v>1</v>
@@ -1577,19 +1567,22 @@
         <v>1</v>
       </c>
       <c r="Q7" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="S7" s="21" t="s">
+      <c r="T7" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="T7" s="21"/>
-      <c r="U7" s="51"/>
-      <c r="V7" s="141"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="51"/>
+      <c r="W7" s="141"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>7</v>
       </c>
@@ -1599,59 +1592,60 @@
       <c r="C8" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>29</v>
-      </c>
+      <c r="D8" s="25"/>
       <c r="E8" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="25" t="s">
+      <c r="G8" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="J8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="N8" s="25" t="s">
-        <v>43</v>
+      <c r="M8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" s="27" t="s">
+        <v>17</v>
       </c>
       <c r="O8" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="R8" s="52" t="s">
+      <c r="P8" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="S8" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="S8" s="25" t="s">
+      <c r="T8" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="T8" s="25"/>
-      <c r="U8" s="52"/>
-      <c r="V8" s="136" t="s">
+      <c r="U8" s="25"/>
+      <c r="V8" s="52"/>
+      <c r="W8" s="136" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>9</v>
       </c>
@@ -1662,60 +1656,63 @@
         <v>99</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E9" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="29" t="s">
+      <c r="G9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="29" t="s">
+      <c r="J9" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="29" t="s">
-        <v>43</v>
+      <c r="M9" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="O9" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="R9" s="53" t="s">
+      <c r="P9" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="S9" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="S9" s="29" t="s">
+      <c r="T9" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="T9" s="29">
+      <c r="U9" s="29">
         <v>1</v>
       </c>
-      <c r="U9" s="53">
+      <c r="V9" s="53">
         <v>0.01</v>
       </c>
-      <c r="V9" s="137"/>
+      <c r="W9" s="137"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>8</v>
       </c>
@@ -1725,38 +1722,36 @@
       <c r="C10" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="33" t="s">
-        <v>29</v>
-      </c>
+      <c r="D10" s="33"/>
       <c r="E10" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="G10" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="33" t="s">
+      <c r="G10" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="33" t="s">
+      <c r="J10" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="33" t="s">
+      <c r="M10" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="35" t="s">
+      <c r="N10" s="35" t="s">
         <v>28</v>
-      </c>
-      <c r="N10" s="33" t="s">
-        <v>43</v>
       </c>
       <c r="O10" s="33" t="s">
         <v>43</v>
@@ -1765,19 +1760,22 @@
         <v>43</v>
       </c>
       <c r="Q10" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="R10" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="R10" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="S10" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="S10" s="33" t="s">
+      <c r="T10" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="T10" s="33"/>
       <c r="U10" s="33"/>
-      <c r="V10" s="138"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="138"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>7</v>
       </c>
@@ -1787,57 +1785,58 @@
       <c r="C11" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="37" t="s">
-        <v>29</v>
-      </c>
+      <c r="D11" s="37"/>
       <c r="E11" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="G11" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="37" t="s">
+      <c r="G11" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="37" t="s">
+      <c r="J11" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="68" t="s">
+      <c r="K11" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="37" t="s">
+      <c r="L11" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="M11" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="N11" s="37" t="s">
+      <c r="M11" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="O11" s="37"/>
       <c r="P11" s="37"/>
-      <c r="Q11" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="R11" s="73" t="s">
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="S11" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="S11" s="37" t="s">
+      <c r="T11" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="T11" s="37"/>
       <c r="U11" s="37"/>
-      <c r="V11" s="160" t="s">
+      <c r="V11" s="37"/>
+      <c r="W11" s="160" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>9</v>
       </c>
@@ -1848,58 +1847,61 @@
         <v>99</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E12" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="41" t="s">
+      <c r="G12" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="41" t="s">
+      <c r="J12" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="L12" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="M12" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="N12" s="41" t="s">
+      <c r="M12" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="O12" s="41"/>
       <c r="P12" s="41"/>
-      <c r="Q12" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="R12" s="54" t="s">
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="S12" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="S12" s="41" t="s">
+      <c r="T12" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="T12" s="41">
+      <c r="U12" s="41">
         <v>1</v>
       </c>
-      <c r="U12" s="54">
+      <c r="V12" s="54">
         <v>0.01</v>
       </c>
-      <c r="V12" s="161"/>
+      <c r="W12" s="161"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
         <v>8</v>
       </c>
@@ -1909,55 +1911,56 @@
       <c r="C13" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="45" t="s">
-        <v>29</v>
-      </c>
+      <c r="D13" s="45"/>
       <c r="E13" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="G13" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="45" t="s">
+      <c r="G13" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="I13" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="45" t="s">
+      <c r="J13" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="L13" s="45" t="s">
+      <c r="M13" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="N13" s="45" t="s">
+      <c r="N13" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="O13" s="45"/>
       <c r="P13" s="45"/>
-      <c r="Q13" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="R13" s="70" t="s">
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="S13" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="S13" s="45" t="s">
+      <c r="T13" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="T13" s="45"/>
       <c r="U13" s="45"/>
-      <c r="V13" s="162"/>
+      <c r="V13" s="45"/>
+      <c r="W13" s="162"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="124" t="s">
         <v>7</v>
       </c>
@@ -1967,57 +1970,58 @@
       <c r="C14" s="125" t="s">
         <v>99</v>
       </c>
-      <c r="D14" s="125" t="s">
-        <v>29</v>
-      </c>
+      <c r="D14" s="125"/>
       <c r="E14" s="125" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="125" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="126" t="s">
-        <v>104</v>
-      </c>
-      <c r="G14" s="127" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="125" t="s">
+      <c r="G14" s="126" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" s="127" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="I14" s="125" t="s">
+      <c r="J14" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="128" t="s">
+      <c r="K14" s="128" t="s">
         <v>46</v>
       </c>
-      <c r="K14" s="125" t="s">
+      <c r="L14" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="L14" s="125" t="s">
-        <v>9</v>
-      </c>
-      <c r="M14" s="128" t="s">
-        <v>17</v>
-      </c>
-      <c r="N14" s="125" t="s">
+      <c r="M14" s="125" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="128" t="s">
+        <v>17</v>
+      </c>
+      <c r="O14" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="O14" s="125"/>
       <c r="P14" s="125"/>
-      <c r="Q14" s="125" t="s">
-        <v>29</v>
-      </c>
+      <c r="Q14" s="125"/>
       <c r="R14" s="125" t="s">
+        <v>29</v>
+      </c>
+      <c r="S14" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="S14" s="125" t="s">
+      <c r="T14" s="125" t="s">
         <v>55</v>
       </c>
-      <c r="T14" s="125"/>
       <c r="U14" s="125"/>
-      <c r="V14" s="154" t="s">
+      <c r="V14" s="125"/>
+      <c r="W14" s="154" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="129" t="s">
         <v>9</v>
       </c>
@@ -2028,58 +2032,61 @@
         <v>99</v>
       </c>
       <c r="D15" s="126" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E15" s="126" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="126" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="130" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="126" t="s">
+      <c r="G15" s="126" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="130" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="126" t="s">
         <v>96</v>
       </c>
-      <c r="I15" s="126" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="131" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15" s="126" t="s">
+      <c r="J15" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="131" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="126" t="s">
         <v>96</v>
       </c>
-      <c r="L15" s="126" t="s">
-        <v>9</v>
-      </c>
-      <c r="M15" s="131" t="s">
-        <v>17</v>
-      </c>
-      <c r="N15" s="126" t="s">
+      <c r="M15" s="126" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" s="131" t="s">
+        <v>17</v>
+      </c>
+      <c r="O15" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="O15" s="126"/>
       <c r="P15" s="126"/>
-      <c r="Q15" s="126" t="s">
-        <v>29</v>
-      </c>
+      <c r="Q15" s="126"/>
       <c r="R15" s="126" t="s">
+        <v>29</v>
+      </c>
+      <c r="S15" s="126" t="s">
         <v>53</v>
       </c>
-      <c r="S15" s="126" t="s">
+      <c r="T15" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="T15" s="126">
+      <c r="U15" s="126">
         <v>1</v>
       </c>
-      <c r="U15" s="126">
+      <c r="V15" s="126">
         <v>0.01</v>
       </c>
-      <c r="V15" s="155"/>
+      <c r="W15" s="155"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="132" t="s">
         <v>8</v>
       </c>
@@ -2089,55 +2096,56 @@
       <c r="C16" s="133" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="133" t="s">
-        <v>29</v>
-      </c>
+      <c r="D16" s="133"/>
       <c r="E16" s="133" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="133" t="s">
-        <v>104</v>
-      </c>
-      <c r="G16" s="134" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="133" t="s">
+      <c r="G16" s="133" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" s="134" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="133" t="s">
         <v>96</v>
       </c>
-      <c r="I16" s="133" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="135" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="133" t="s">
+      <c r="J16" s="133" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="135" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="133" t="s">
         <v>96</v>
       </c>
-      <c r="L16" s="133" t="s">
+      <c r="M16" s="133" t="s">
         <v>80</v>
       </c>
-      <c r="M16" s="135" t="s">
-        <v>17</v>
-      </c>
-      <c r="N16" s="133" t="s">
+      <c r="N16" s="135" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16" s="133" t="s">
         <v>47</v>
       </c>
-      <c r="O16" s="133"/>
       <c r="P16" s="133"/>
-      <c r="Q16" s="133" t="s">
-        <v>29</v>
-      </c>
+      <c r="Q16" s="133"/>
       <c r="R16" s="133" t="s">
+        <v>29</v>
+      </c>
+      <c r="S16" s="133" t="s">
         <v>54</v>
       </c>
-      <c r="S16" s="133" t="s">
+      <c r="T16" s="133" t="s">
         <v>55</v>
       </c>
-      <c r="T16" s="133"/>
       <c r="U16" s="133"/>
-      <c r="V16" s="156"/>
+      <c r="V16" s="133"/>
+      <c r="W16" s="156"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
         <v>7</v>
       </c>
@@ -2147,57 +2155,58 @@
       <c r="C17" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="56" t="s">
-        <v>29</v>
-      </c>
+      <c r="D17" s="56"/>
       <c r="E17" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="57" t="s">
-        <v>105</v>
-      </c>
-      <c r="G17" s="58" t="s">
+      <c r="G17" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="H17" s="56" t="s">
+      <c r="I17" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="I17" s="56" t="s">
+      <c r="J17" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="J17" s="69" t="s">
+      <c r="K17" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="K17" s="56" t="s">
+      <c r="L17" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="L17" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="M17" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="N17" s="56" t="s">
+      <c r="M17" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="O17" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="O17" s="56"/>
       <c r="P17" s="56"/>
-      <c r="Q17" s="56" t="s">
-        <v>29</v>
-      </c>
-      <c r="R17" s="74" t="s">
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="S17" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="S17" s="56" t="s">
+      <c r="T17" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="T17" s="56"/>
       <c r="U17" s="56"/>
-      <c r="V17" s="145" t="s">
+      <c r="V17" s="56"/>
+      <c r="W17" s="145" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="s">
         <v>9</v>
       </c>
@@ -2208,58 +2217,61 @@
         <v>99</v>
       </c>
       <c r="D18" s="57" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E18" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="61" t="s">
+      <c r="G18" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="57" t="s">
+      <c r="I18" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="I18" s="57" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="57" t="s">
+      <c r="J18" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="L18" s="57" t="s">
-        <v>9</v>
-      </c>
-      <c r="M18" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="N18" s="57" t="s">
+      <c r="M18" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="O18" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="O18" s="57"/>
       <c r="P18" s="57"/>
-      <c r="Q18" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="R18" s="63" t="s">
+      <c r="Q18" s="57"/>
+      <c r="R18" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="S18" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="S18" s="57" t="s">
+      <c r="T18" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="T18" s="57">
+      <c r="U18" s="57">
         <v>1</v>
       </c>
-      <c r="U18" s="63">
+      <c r="V18" s="63">
         <v>0.01</v>
       </c>
-      <c r="V18" s="146"/>
+      <c r="W18" s="146"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="64" t="s">
         <v>8</v>
       </c>
@@ -2269,55 +2281,56 @@
       <c r="C19" s="65" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="65" t="s">
-        <v>29</v>
-      </c>
+      <c r="D19" s="65"/>
       <c r="E19" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="G19" s="66" t="s">
+      <c r="G19" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="H19" s="65" t="s">
+      <c r="I19" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="I19" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" s="65" t="s">
+      <c r="J19" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="L19" s="65" t="s">
+      <c r="M19" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="M19" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="N19" s="65" t="s">
+      <c r="N19" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="O19" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="O19" s="65"/>
       <c r="P19" s="65"/>
-      <c r="Q19" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="R19" s="75" t="s">
+      <c r="Q19" s="65"/>
+      <c r="R19" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="S19" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="S19" s="65" t="s">
+      <c r="T19" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="T19" s="65"/>
       <c r="U19" s="65"/>
-      <c r="V19" s="147"/>
+      <c r="V19" s="65"/>
+      <c r="W19" s="147"/>
     </row>
-    <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="76" t="s">
         <v>7</v>
       </c>
@@ -2327,57 +2340,58 @@
       <c r="C20" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="77" t="s">
-        <v>29</v>
-      </c>
+      <c r="D20" s="77"/>
       <c r="E20" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="78" t="s">
-        <v>106</v>
-      </c>
-      <c r="G20" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="77" t="s">
+      <c r="G20" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="I20" s="77" t="s">
+      <c r="J20" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="80" t="s">
+      <c r="K20" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="K20" s="77" t="s">
+      <c r="L20" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="L20" s="77" t="s">
-        <v>9</v>
-      </c>
-      <c r="M20" s="81" t="s">
-        <v>17</v>
-      </c>
-      <c r="N20" s="77" t="s">
+      <c r="M20" s="77" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" s="81" t="s">
+        <v>17</v>
+      </c>
+      <c r="O20" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="O20" s="77"/>
       <c r="P20" s="77"/>
-      <c r="Q20" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="R20" s="82" t="s">
+      <c r="Q20" s="77"/>
+      <c r="R20" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="S20" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="S20" s="77" t="s">
+      <c r="T20" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="T20" s="77"/>
       <c r="U20" s="77"/>
-      <c r="V20" s="148" t="s">
+      <c r="V20" s="77"/>
+      <c r="W20" s="148" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="83" t="s">
         <v>9</v>
       </c>
@@ -2388,58 +2402,61 @@
         <v>99</v>
       </c>
       <c r="D21" s="78" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E21" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="84" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="78" t="s">
+      <c r="G21" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="84" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="I21" s="78" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" s="85" t="s">
-        <v>17</v>
-      </c>
-      <c r="K21" s="78" t="s">
+      <c r="J21" s="78" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="L21" s="78" t="s">
-        <v>9</v>
-      </c>
-      <c r="M21" s="85" t="s">
-        <v>17</v>
-      </c>
-      <c r="N21" s="78" t="s">
+      <c r="M21" s="78" t="s">
+        <v>9</v>
+      </c>
+      <c r="N21" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="O21" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="O21" s="78"/>
       <c r="P21" s="78"/>
-      <c r="Q21" s="78" t="s">
-        <v>29</v>
-      </c>
-      <c r="R21" s="86" t="s">
+      <c r="Q21" s="78"/>
+      <c r="R21" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="S21" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="S21" s="78" t="s">
+      <c r="T21" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="T21" s="78">
+      <c r="U21" s="78">
         <v>1</v>
       </c>
-      <c r="U21" s="86">
+      <c r="V21" s="86">
         <v>0.01</v>
       </c>
-      <c r="V21" s="149"/>
+      <c r="W21" s="149"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="87" t="s">
         <v>8</v>
       </c>
@@ -2449,57 +2466,58 @@
       <c r="C22" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="88" t="s">
-        <v>29</v>
-      </c>
+      <c r="D22" s="88"/>
       <c r="E22" s="88" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="88" t="s">
-        <v>106</v>
-      </c>
-      <c r="G22" s="89" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="88" t="s">
+      <c r="G22" s="88" t="s">
+        <v>72</v>
+      </c>
+      <c r="H22" s="89" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="88" t="s">
         <v>74</v>
       </c>
-      <c r="I22" s="88" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" s="90" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="88" t="s">
+      <c r="J22" s="88" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="L22" s="88" t="s">
+      <c r="M22" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="M22" s="90" t="s">
-        <v>17</v>
-      </c>
-      <c r="N22" s="88" t="s">
+      <c r="N22" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="O22" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="O22" s="88"/>
-      <c r="P22" s="88" t="s">
+      <c r="P22" s="88"/>
+      <c r="Q22" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="Q22" s="88" t="s">
-        <v>29</v>
-      </c>
-      <c r="R22" s="91" t="s">
+      <c r="R22" s="88" t="s">
+        <v>29</v>
+      </c>
+      <c r="S22" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="S22" s="88" t="s">
+      <c r="T22" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="T22" s="88"/>
       <c r="U22" s="88"/>
-      <c r="V22" s="150"/>
+      <c r="V22" s="88"/>
+      <c r="W22" s="150"/>
     </row>
-    <row r="23" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="92" t="s">
         <v>7</v>
       </c>
@@ -2509,57 +2527,58 @@
       <c r="C23" s="93" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="93" t="s">
-        <v>29</v>
-      </c>
+      <c r="D23" s="93"/>
       <c r="E23" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="94" t="s">
-        <v>107</v>
-      </c>
-      <c r="G23" s="95" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" s="93" t="s">
+      <c r="G23" s="94" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="95" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="I23" s="93" t="s">
+      <c r="J23" s="93" t="s">
         <v>80</v>
       </c>
-      <c r="J23" s="96" t="s">
-        <v>17</v>
-      </c>
-      <c r="K23" s="93" t="s">
+      <c r="K23" s="96" t="s">
+        <v>17</v>
+      </c>
+      <c r="L23" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="L23" s="93" t="s">
-        <v>9</v>
-      </c>
-      <c r="M23" s="97" t="s">
-        <v>17</v>
-      </c>
-      <c r="N23" s="93" t="s">
+      <c r="M23" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="N23" s="97" t="s">
+        <v>17</v>
+      </c>
+      <c r="O23" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="O23" s="93"/>
       <c r="P23" s="93"/>
-      <c r="Q23" s="93" t="s">
-        <v>29</v>
-      </c>
-      <c r="R23" s="98" t="s">
+      <c r="Q23" s="93"/>
+      <c r="R23" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="S23" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="S23" s="93" t="s">
+      <c r="T23" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="T23" s="93"/>
       <c r="U23" s="93"/>
-      <c r="V23" s="151" t="s">
+      <c r="V23" s="93"/>
+      <c r="W23" s="151" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="99" t="s">
         <v>9</v>
       </c>
@@ -2570,58 +2589,61 @@
         <v>99</v>
       </c>
       <c r="D24" s="94" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E24" s="94" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="94" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="100" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" s="94" t="s">
+      <c r="G24" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="100" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="I24" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="J24" s="101" t="s">
-        <v>17</v>
-      </c>
-      <c r="K24" s="94" t="s">
+      <c r="J24" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="K24" s="101" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="L24" s="94" t="s">
-        <v>9</v>
-      </c>
-      <c r="M24" s="101" t="s">
-        <v>17</v>
-      </c>
-      <c r="N24" s="94" t="s">
+      <c r="M24" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="N24" s="101" t="s">
+        <v>17</v>
+      </c>
+      <c r="O24" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="O24" s="94"/>
       <c r="P24" s="94"/>
-      <c r="Q24" s="94" t="s">
-        <v>29</v>
-      </c>
-      <c r="R24" s="102" t="s">
+      <c r="Q24" s="94"/>
+      <c r="R24" s="94" t="s">
+        <v>29</v>
+      </c>
+      <c r="S24" s="102" t="s">
         <v>54</v>
       </c>
-      <c r="S24" s="94" t="s">
+      <c r="T24" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="T24" s="94">
+      <c r="U24" s="94">
         <v>1</v>
       </c>
-      <c r="U24" s="102">
+      <c r="V24" s="102">
         <v>0.01</v>
       </c>
-      <c r="V24" s="152"/>
+      <c r="W24" s="152"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="103" t="s">
         <v>8</v>
       </c>
@@ -2631,57 +2653,58 @@
       <c r="C25" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="104" t="s">
-        <v>29</v>
-      </c>
+      <c r="D25" s="104"/>
       <c r="E25" s="104" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="104" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" s="105" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" s="104" t="s">
+      <c r="G25" s="104" t="s">
+        <v>83</v>
+      </c>
+      <c r="H25" s="105" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="I25" s="104" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25" s="106" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" s="104" t="s">
+      <c r="J25" s="104" t="s">
+        <v>9</v>
+      </c>
+      <c r="K25" s="106" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="L25" s="104" t="s">
+      <c r="M25" s="104" t="s">
         <v>80</v>
       </c>
-      <c r="M25" s="106" t="s">
-        <v>17</v>
-      </c>
-      <c r="N25" s="104" t="s">
+      <c r="N25" s="106" t="s">
+        <v>17</v>
+      </c>
+      <c r="O25" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="O25" s="104"/>
-      <c r="P25" s="104" t="s">
+      <c r="P25" s="104"/>
+      <c r="Q25" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="Q25" s="104" t="s">
-        <v>29</v>
-      </c>
-      <c r="R25" s="107" t="s">
+      <c r="R25" s="104" t="s">
+        <v>29</v>
+      </c>
+      <c r="S25" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="S25" s="104" t="s">
+      <c r="T25" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="T25" s="104"/>
       <c r="U25" s="104"/>
-      <c r="V25" s="153"/>
+      <c r="V25" s="104"/>
+      <c r="W25" s="153"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="108" t="s">
         <v>7</v>
       </c>
@@ -2691,57 +2714,58 @@
       <c r="C26" s="109" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="109" t="s">
-        <v>29</v>
-      </c>
+      <c r="D26" s="109"/>
       <c r="E26" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="109" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="110" t="s">
-        <v>108</v>
-      </c>
-      <c r="G26" s="111" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="109" t="s">
+      <c r="G26" s="110" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" s="111" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="109" t="s">
         <v>88</v>
       </c>
-      <c r="I26" s="109" t="s">
+      <c r="J26" s="109" t="s">
         <v>80</v>
       </c>
-      <c r="J26" s="112" t="s">
-        <v>17</v>
-      </c>
-      <c r="K26" s="109" t="s">
+      <c r="K26" s="112" t="s">
+        <v>17</v>
+      </c>
+      <c r="L26" s="109" t="s">
         <v>88</v>
       </c>
-      <c r="L26" s="109" t="s">
-        <v>9</v>
-      </c>
-      <c r="M26" s="113" t="s">
-        <v>17</v>
-      </c>
-      <c r="N26" s="109" t="s">
+      <c r="M26" s="109" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="O26" s="109" t="s">
         <v>69</v>
       </c>
-      <c r="O26" s="109"/>
       <c r="P26" s="109"/>
-      <c r="Q26" s="109" t="s">
-        <v>29</v>
-      </c>
-      <c r="R26" s="114" t="s">
+      <c r="Q26" s="109"/>
+      <c r="R26" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="S26" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="S26" s="109" t="s">
+      <c r="T26" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="T26" s="109"/>
       <c r="U26" s="109"/>
-      <c r="V26" s="157" t="s">
+      <c r="V26" s="109"/>
+      <c r="W26" s="157" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="115" t="s">
         <v>9</v>
       </c>
@@ -2752,58 +2776,61 @@
         <v>99</v>
       </c>
       <c r="D27" s="110" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E27" s="110" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="110" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="116" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="110" t="s">
+      <c r="G27" s="110" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="116" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="110" t="s">
         <v>88</v>
       </c>
-      <c r="I27" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="J27" s="117" t="s">
-        <v>17</v>
-      </c>
-      <c r="K27" s="110" t="s">
+      <c r="J27" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="K27" s="117" t="s">
+        <v>17</v>
+      </c>
+      <c r="L27" s="110" t="s">
         <v>88</v>
       </c>
-      <c r="L27" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="M27" s="117" t="s">
-        <v>17</v>
-      </c>
-      <c r="N27" s="110" t="s">
+      <c r="M27" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="N27" s="117" t="s">
+        <v>17</v>
+      </c>
+      <c r="O27" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="O27" s="110"/>
       <c r="P27" s="110"/>
-      <c r="Q27" s="110" t="s">
-        <v>29</v>
-      </c>
-      <c r="R27" s="118" t="s">
+      <c r="Q27" s="110"/>
+      <c r="R27" s="110" t="s">
+        <v>29</v>
+      </c>
+      <c r="S27" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="S27" s="110" t="s">
+      <c r="T27" s="110" t="s">
         <v>77</v>
       </c>
-      <c r="T27" s="110">
+      <c r="U27" s="110">
         <v>1</v>
       </c>
-      <c r="U27" s="118">
+      <c r="V27" s="118">
         <v>0.01</v>
       </c>
-      <c r="V27" s="158"/>
+      <c r="W27" s="158"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="119" t="s">
         <v>8</v>
       </c>
@@ -2813,67 +2840,68 @@
       <c r="C28" s="120" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="120" t="s">
-        <v>29</v>
-      </c>
+      <c r="D28" s="120"/>
       <c r="E28" s="120" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="120" t="s">
-        <v>108</v>
-      </c>
-      <c r="G28" s="121" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="120" t="s">
+      <c r="G28" s="120" t="s">
+        <v>86</v>
+      </c>
+      <c r="H28" s="121" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="120" t="s">
         <v>88</v>
       </c>
-      <c r="I28" s="120" t="s">
-        <v>9</v>
-      </c>
-      <c r="J28" s="122" t="s">
-        <v>17</v>
-      </c>
-      <c r="K28" s="120" t="s">
+      <c r="J28" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="K28" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="120" t="s">
         <v>88</v>
       </c>
-      <c r="L28" s="120" t="s">
+      <c r="M28" s="120" t="s">
         <v>80</v>
       </c>
-      <c r="M28" s="122" t="s">
-        <v>17</v>
-      </c>
-      <c r="N28" s="120" t="s">
+      <c r="N28" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="O28" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="O28" s="120"/>
-      <c r="P28" s="120" t="s">
+      <c r="P28" s="120"/>
+      <c r="Q28" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="Q28" s="120" t="s">
-        <v>29</v>
-      </c>
-      <c r="R28" s="123" t="s">
+      <c r="R28" s="120" t="s">
+        <v>29</v>
+      </c>
+      <c r="S28" s="123" t="s">
         <v>52</v>
       </c>
-      <c r="S28" s="120" t="s">
+      <c r="T28" s="120" t="s">
         <v>77</v>
       </c>
-      <c r="T28" s="120"/>
       <c r="U28" s="120"/>
-      <c r="V28" s="159"/>
+      <c r="V28" s="120"/>
+      <c r="W28" s="159"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="V23:V25"/>
-    <mergeCell ref="V14:V16"/>
-    <mergeCell ref="V26:V28"/>
-    <mergeCell ref="V11:V13"/>
-    <mergeCell ref="V8:V10"/>
-    <mergeCell ref="V5:V7"/>
-    <mergeCell ref="V2:V4"/>
-    <mergeCell ref="V17:V19"/>
-    <mergeCell ref="V20:V22"/>
+    <mergeCell ref="W23:W25"/>
+    <mergeCell ref="W14:W16"/>
+    <mergeCell ref="W26:W28"/>
+    <mergeCell ref="W11:W13"/>
+    <mergeCell ref="W8:W10"/>
+    <mergeCell ref="W5:W7"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="W17:W19"/>
+    <mergeCell ref="W20:W22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>